<commit_message>
Finally add alll the minutes and Papers I said I would Many Weeks Ago
</commit_message>
<xml_diff>
--- a/Hani/Sensors/SensorComparisons.xlsx
+++ b/Hani/Sensors/SensorComparisons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanim\Desktop\Sims\Degree\CubeSat_project\Hani\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanim\Desktop\Sims\Degree\CubeSat_project\Hani\Sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF24ACB-4561-4DAA-9E92-BAD04274982B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E211E6-D429-4749-9BEB-C5726100DD6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="86">
   <si>
     <t>Source</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Acoustic Emission has no heritage</t>
+  </si>
+  <si>
+    <t>https://www.ameteksfms.com/-/media/ameteksensors/documents/sensor%20data%20sheets/pressure-transducers-thin-film.pdf</t>
   </si>
 </sst>
 </file>
@@ -384,11 +387,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -670,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,7 +718,7 @@
       <c r="J1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -724,7 +727,7 @@
       <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -733,16 +736,16 @@
       <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="8"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -751,7 +754,7 @@
       <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -760,7 +763,7 @@
       <c r="F3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>31</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -771,7 +774,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -797,7 +800,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -806,7 +809,7 @@
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -826,7 +829,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -855,7 +858,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -864,7 +867,7 @@
       <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -884,7 +887,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -893,7 +896,7 @@
       <c r="C8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -913,7 +916,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -939,7 +942,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>64</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -965,7 +968,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -991,7 +994,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1000,7 +1003,7 @@
       <c r="C12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>75</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -1017,7 +1020,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1026,7 +1029,7 @@
       <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>78</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1035,7 +1038,7 @@
       <c r="F13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>80</v>
       </c>
       <c r="I13" s="6" t="s">
@@ -1046,7 +1049,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1066,6 +1069,17 @@
       </c>
       <c r="G14" s="1" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1100,8 +1114,9 @@
     <hyperlink ref="A13" r:id="rId25" xr:uid="{CDB280A9-0D22-47F4-BAFB-5E9D10CAFAE7}"/>
     <hyperlink ref="G13" r:id="rId26" xr:uid="{4830564B-FFE7-40AE-99AD-41E0187849C1}"/>
     <hyperlink ref="A14" r:id="rId27" xr:uid="{4AE1237B-A8F7-4D74-824B-5CD3BAA4DE23}"/>
+    <hyperlink ref="A15" r:id="rId28" xr:uid="{F6F6513B-F7EE-4DB7-9268-173F90AA06B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>